<commit_message>
auditoria revision no conformidades
</commit_message>
<xml_diff>
--- a/Proyectos/2016/1/P1433 - RNCFAC2, Alejandro Martinez_MO/Calidad/No_conformidades.xlsx
+++ b/Proyectos/2016/1/P1433 - RNCFAC2, Alejandro Martinez_MO/Calidad/No_conformidades.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
   <si>
     <t>REPORTE DE NO CONFORMIDADES P1433 - RNCFAC2, Alejandro Martinez_MO</t>
   </si>
@@ -47,7 +47,7 @@
     <t>Marisol Ornelas</t>
   </si>
   <si>
-    <t>En proceso</t>
+    <t>Cerrada</t>
   </si>
   <si>
     <t>Crear una carpeta llamada lineabase y agregar tambien el plan de proyecto, carta de aceptacion, estimacion y cotizacion.</t>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>Judith Jaramillo</t>
+  </si>
+  <si>
+    <t>N/a</t>
   </si>
   <si>
     <t>Generar encuesta de satisfaccion</t>
@@ -319,7 +322,7 @@
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -391,7 +394,9 @@
       <c r="D4" s="5" t="n">
         <v>42397</v>
       </c>
-      <c r="E4" s="5"/>
+      <c r="E4" s="5" t="n">
+        <v>42397</v>
+      </c>
       <c r="F4" s="6" t="s">
         <v>10</v>
       </c>
@@ -412,7 +417,9 @@
       <c r="D5" s="5" t="n">
         <v>42397</v>
       </c>
-      <c r="E5" s="5"/>
+      <c r="E5" s="5" t="n">
+        <v>42397</v>
+      </c>
       <c r="F5" s="6" t="s">
         <v>10</v>
       </c>
@@ -433,12 +440,14 @@
       <c r="D6" s="5" t="n">
         <v>42397</v>
       </c>
-      <c r="E6" s="5"/>
+      <c r="E6" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="F6" s="6" t="s">
         <v>10</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -446,7 +455,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>9</v>
@@ -454,7 +463,9 @@
       <c r="D7" s="5" t="n">
         <v>42397</v>
       </c>
-      <c r="E7" s="5"/>
+      <c r="E7" s="5" t="n">
+        <v>42397</v>
+      </c>
       <c r="F7" s="6" t="s">
         <v>10</v>
       </c>
@@ -465,7 +476,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>9</v>
@@ -473,7 +484,9 @@
       <c r="D8" s="5" t="n">
         <v>42397</v>
       </c>
-      <c r="E8" s="5"/>
+      <c r="E8" s="5" t="n">
+        <v>42397</v>
+      </c>
       <c r="F8" s="6" t="s">
         <v>10</v>
       </c>
@@ -484,7 +497,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>9</v>
@@ -492,7 +505,9 @@
       <c r="D9" s="5" t="n">
         <v>42397</v>
       </c>
-      <c r="E9" s="5"/>
+      <c r="E9" s="5" t="n">
+        <v>42397</v>
+      </c>
       <c r="F9" s="6" t="s">
         <v>10</v>
       </c>

</xml_diff>